<commit_message>
20200104 13:37 Final changes applied ready for submission!
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestData.xlsx
+++ b/src/test/resources/data/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramaz\IdeaProjects\GroupProjects\RhytmOfIntegers\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8056E047-CAEE-472E-B087-F7FA0CD6BF30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A901BB1-D12A-451C-8FF3-4BF6FEB4B385}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{A364498F-E2B9-4213-8BA3-B5D83DB6A0B5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A364498F-E2B9-4213-8BA3-B5D83DB6A0B5}"/>
   </bookViews>
   <sheets>
     <sheet name="TC_0001" sheetId="3" r:id="rId1"/>
@@ -118,9 +118,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,61 +443,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{568BD27D-838F-4B82-83C8-2EFDE4E457DB}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="134.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="132.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="83" style="2" customWidth="1"/>
+    <col min="2" max="2" width="77" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -503,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C7ACC3-CF38-4D99-939E-570D18E9F9F2}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
20210104 14:51 Excel file had been updated
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestData.xlsx
+++ b/src/test/resources/data/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramaz\IdeaProjects\GroupProjects\RhytmOfIntegers\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A901BB1-D12A-451C-8FF3-4BF6FEB4B385}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A757557-C92F-4AE2-ACF9-73A15A84A1EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A364498F-E2B9-4213-8BA3-B5D83DB6A0B5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{A364498F-E2B9-4213-8BA3-B5D83DB6A0B5}"/>
   </bookViews>
   <sheets>
     <sheet name="TC_0001" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>sentence</t>
   </si>
@@ -70,9 +70,6 @@
     <t>solutions</t>
   </si>
   <si>
-    <t>In,InRhythm,High,Impact,Teams,embedded,in,your,culture</t>
-  </si>
-  <si>
     <t>An,increase,of,technical,debt,prevents,you,from,growing,your,business</t>
   </si>
   <si>
@@ -83,6 +80,27 @@
   </si>
   <si>
     <t>?? !! ???</t>
+  </si>
+  <si>
+    <t>Google Ads is an online advertising platform developed by Google, where advertisers bid to display brief advertisements, service offerings, product listings, or videos to web users. It can place ads both in the results of search engines like Google Search and on non-search websites, mobile apps, and videos.</t>
+  </si>
+  <si>
+    <t>Google,Ads,is,an,online,advertising,platform,developed,by,Google,where,advertisers,bid,to,display,brief,advertisements,service,offerings,product,listings,or,videos,to,web,users,It,can,place,ads,both,in,the,results,of,search,engines,like,Google,Search,and,on,non-search,websites,mobile,apps,and,videos.</t>
+  </si>
+  <si>
+    <t>Facebook, Inc. is an American technology conglomerate based in Menlo Park, California. It was founded by Mark Zuckerberg, along with his fellow roommates and students at Harvard College, who were Eduardo Saverin, Andrew McCollum, Dustin Moskovitz and Chris Hughes, originally as TheFacebook.com—today's Facebook, a popular global social networking service. Facebook is one of the world's most valuable companies. It is considered one of the Big Five companies in the U.S. information technology industry, along with Google, Apple, Microsoft, and Amazon.</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>Facebook,Inc,is,an,American,technology,conglomerate,based,in,Menlo,Park,California,It,was,founded,by,Mark,Zuckerberg,along,with,his,fellow,roommates,and,students,at,Harvard,College,who,were,Eduardo,Saverin,Andrew,McCollum,Dustin,Moskovitz,and,Chris,Hughes,originally,as,TheFacebook,com—today,s,Facebook,a,popular,global,social,networking,service,Facebook,is,one,of,the,world,s,most,valuable,companies,It,is,considered,one,of,the,Big,Five,companies,in,the,U,S,information,technology,industry,along,with,Google,Apple,Microsoft,and,Amazon</t>
+  </si>
+  <si>
+    <t>conglomerate</t>
+  </si>
+  <si>
+    <t>advertisements</t>
   </si>
 </sst>
 </file>
@@ -441,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{568BD27D-838F-4B82-83C8-2EFDE4E457DB}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,43 +479,59 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="3"/>
+      <c r="B8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -507,10 +541,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C7ACC3-CF38-4D99-939E-570D18E9F9F2}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,55 +565,77 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1">
-        <v>8</v>
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2">
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
-        <v>9</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2">
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>